<commit_message>
new features in datanalysis.py
</commit_message>
<xml_diff>
--- a/world-data-2023.xlsx
+++ b/world-data-2023.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2239" uniqueCount="1660">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2064" uniqueCount="1529">
   <si>
     <t>Country</t>
   </si>
@@ -101,7 +101,7 @@
     <t>Population</t>
   </si>
   <si>
-    <t>Population: Labor force participation (%)</t>
+    <t>Labor force participation (%)</t>
   </si>
   <si>
     <t>Tax revenue (%)</t>
@@ -4602,399 +4602,6 @@
   </si>
   <si>
     <t>25.80%</t>
-  </si>
-  <si>
-    <t>48.90%</t>
-  </si>
-  <si>
-    <t>55.70%</t>
-  </si>
-  <si>
-    <t>41.20%</t>
-  </si>
-  <si>
-    <t>77.50%</t>
-  </si>
-  <si>
-    <t>55.60%</t>
-  </si>
-  <si>
-    <t>65.50%</t>
-  </si>
-  <si>
-    <t>60.70%</t>
-  </si>
-  <si>
-    <t>74.60%</t>
-  </si>
-  <si>
-    <t>73.40%</t>
-  </si>
-  <si>
-    <t>59.00%</t>
-  </si>
-  <si>
-    <t>65.20%</t>
-  </si>
-  <si>
-    <t>64.10%</t>
-  </si>
-  <si>
-    <t>53.60%</t>
-  </si>
-  <si>
-    <t>70.90%</t>
-  </si>
-  <si>
-    <t>66.70%</t>
-  </si>
-  <si>
-    <t>46.40%</t>
-  </si>
-  <si>
-    <t>70.80%</t>
-  </si>
-  <si>
-    <t>63.90%</t>
-  </si>
-  <si>
-    <t>64.70%</t>
-  </si>
-  <si>
-    <t>55.40%</t>
-  </si>
-  <si>
-    <t>66.40%</t>
-  </si>
-  <si>
-    <t>79.20%</t>
-  </si>
-  <si>
-    <t>60.50%</t>
-  </si>
-  <si>
-    <t>82.30%</t>
-  </si>
-  <si>
-    <t>76.10%</t>
-  </si>
-  <si>
-    <t>70.70%</t>
-  </si>
-  <si>
-    <t>62.60%</t>
-  </si>
-  <si>
-    <t>68.00%</t>
-  </si>
-  <si>
-    <t>68.80%</t>
-  </si>
-  <si>
-    <t>43.30%</t>
-  </si>
-  <si>
-    <t>69.40%</t>
-  </si>
-  <si>
-    <t>62.10%</t>
-  </si>
-  <si>
-    <t>51.20%</t>
-  </si>
-  <si>
-    <t>60.60%</t>
-  </si>
-  <si>
-    <t>63.50%</t>
-  </si>
-  <si>
-    <t>62.20%</t>
-  </si>
-  <si>
-    <t>60.20%</t>
-  </si>
-  <si>
-    <t>64.30%</t>
-  </si>
-  <si>
-    <t>59.10%</t>
-  </si>
-  <si>
-    <t>63.60%</t>
-  </si>
-  <si>
-    <t>79.60%</t>
-  </si>
-  <si>
-    <t>57.60%</t>
-  </si>
-  <si>
-    <t>55.10%</t>
-  </si>
-  <si>
-    <t>52.90%</t>
-  </si>
-  <si>
-    <t>68.30%</t>
-  </si>
-  <si>
-    <t>60.80%</t>
-  </si>
-  <si>
-    <t>67.80%</t>
-  </si>
-  <si>
-    <t>51.80%</t>
-  </si>
-  <si>
-    <t>62.30%</t>
-  </si>
-  <si>
-    <t>61.50%</t>
-  </si>
-  <si>
-    <t>56.20%</t>
-  </si>
-  <si>
-    <t>67.20%</t>
-  </si>
-  <si>
-    <t>56.50%</t>
-  </si>
-  <si>
-    <t>75.00%</t>
-  </si>
-  <si>
-    <t>49.30%</t>
-  </si>
-  <si>
-    <t>67.50%</t>
-  </si>
-  <si>
-    <t>44.70%</t>
-  </si>
-  <si>
-    <t>43.00%</t>
-  </si>
-  <si>
-    <t>64.00%</t>
-  </si>
-  <si>
-    <t>49.60%</t>
-  </si>
-  <si>
-    <t>66.00%</t>
-  </si>
-  <si>
-    <t>61.70%</t>
-  </si>
-  <si>
-    <t>74.70%</t>
-  </si>
-  <si>
-    <t>73.50%</t>
-  </si>
-  <si>
-    <t>59.80%</t>
-  </si>
-  <si>
-    <t>78.50%</t>
-  </si>
-  <si>
-    <t>61.40%</t>
-  </si>
-  <si>
-    <t>47.00%</t>
-  </si>
-  <si>
-    <t>67.90%</t>
-  </si>
-  <si>
-    <t>76.30%</t>
-  </si>
-  <si>
-    <t>49.70%</t>
-  </si>
-  <si>
-    <t>61.60%</t>
-  </si>
-  <si>
-    <t>59.30%</t>
-  </si>
-  <si>
-    <t>86.10%</t>
-  </si>
-  <si>
-    <t>76.70%</t>
-  </si>
-  <si>
-    <t>69.80%</t>
-  </si>
-  <si>
-    <t>45.90%</t>
-  </si>
-  <si>
-    <t>58.30%</t>
-  </si>
-  <si>
-    <t>43.10%</t>
-  </si>
-  <si>
-    <t>59.70%</t>
-  </si>
-  <si>
-    <t>54.40%</t>
-  </si>
-  <si>
-    <t>45.30%</t>
-  </si>
-  <si>
-    <t>78.10%</t>
-  </si>
-  <si>
-    <t>59.50%</t>
-  </si>
-  <si>
-    <t>83.80%</t>
-  </si>
-  <si>
-    <t>69.90%</t>
-  </si>
-  <si>
-    <t>80.40%</t>
-  </si>
-  <si>
-    <t>63.80%</t>
-  </si>
-  <si>
-    <t>72.40%</t>
-  </si>
-  <si>
-    <t>52.60%</t>
-  </si>
-  <si>
-    <t>66.60%</t>
-  </si>
-  <si>
-    <t>47.20%</t>
-  </si>
-  <si>
-    <t>72.10%</t>
-  </si>
-  <si>
-    <t>77.60%</t>
-  </si>
-  <si>
-    <t>59.60%</t>
-  </si>
-  <si>
-    <t>56.70%</t>
-  </si>
-  <si>
-    <t>58.80%</t>
-  </si>
-  <si>
-    <t>86.80%</t>
-  </si>
-  <si>
-    <t>54.70%</t>
-  </si>
-  <si>
-    <t>61.80%</t>
-  </si>
-  <si>
-    <t>83.70%</t>
-  </si>
-  <si>
-    <t>67.10%</t>
-  </si>
-  <si>
-    <t>65.90%</t>
-  </si>
-  <si>
-    <t>55.90%</t>
-  </si>
-  <si>
-    <t>45.70%</t>
-  </si>
-  <si>
-    <t>54.90%</t>
-  </si>
-  <si>
-    <t>57.90%</t>
-  </si>
-  <si>
-    <t>70.50%</t>
-  </si>
-  <si>
-    <t>58.40%</t>
-  </si>
-  <si>
-    <t>47.40%</t>
-  </si>
-  <si>
-    <t>56.00%</t>
-  </si>
-  <si>
-    <t>63.00%</t>
-  </si>
-  <si>
-    <t>57.50%</t>
-  </si>
-  <si>
-    <t>53.90%</t>
-  </si>
-  <si>
-    <t>51.10%</t>
-  </si>
-  <si>
-    <t>64.60%</t>
-  </si>
-  <si>
-    <t>44.10%</t>
-  </si>
-  <si>
-    <t>42.00%</t>
-  </si>
-  <si>
-    <t>83.40%</t>
-  </si>
-  <si>
-    <t>67.30%</t>
-  </si>
-  <si>
-    <t>60.00%</t>
-  </si>
-  <si>
-    <t>46.10%</t>
-  </si>
-  <si>
-    <t>52.80%</t>
-  </si>
-  <si>
-    <t>64.50%</t>
-  </si>
-  <si>
-    <t>70.30%</t>
-  </si>
-  <si>
-    <t>54.20%</t>
-  </si>
-  <si>
-    <t>82.10%</t>
-  </si>
-  <si>
-    <t>62.80%</t>
-  </si>
-  <si>
-    <t>77.40%</t>
-  </si>
-  <si>
-    <t>38.00%</t>
-  </si>
-  <si>
-    <t>83.10%</t>
   </si>
 </sst>
 </file>
@@ -5553,8 +5160,8 @@
       <c r="AB2">
         <v>38041754</v>
       </c>
-      <c r="AC2" t="s">
-        <v>1529</v>
+      <c r="AC2">
+        <v>48.9</v>
       </c>
       <c r="AD2">
         <v>9.300000000000001</v>
@@ -5663,8 +5270,8 @@
       <c r="AB3">
         <v>2854191</v>
       </c>
-      <c r="AC3" t="s">
-        <v>1530</v>
+      <c r="AC3">
+        <v>55.7</v>
       </c>
       <c r="AD3">
         <v>18.6</v>
@@ -5773,8 +5380,8 @@
       <c r="AB4">
         <v>43053054</v>
       </c>
-      <c r="AC4" t="s">
-        <v>1531</v>
+      <c r="AC4">
+        <v>41.2</v>
       </c>
       <c r="AD4">
         <v>37.2</v>
@@ -5963,8 +5570,8 @@
       <c r="AB6">
         <v>31825295</v>
       </c>
-      <c r="AC6" t="s">
-        <v>1532</v>
+      <c r="AC6">
+        <v>77.5</v>
       </c>
       <c r="AD6">
         <v>9.199999999999999</v>
@@ -6177,8 +5784,8 @@
       <c r="AB8">
         <v>44938712</v>
       </c>
-      <c r="AC8" t="s">
-        <v>1503</v>
+      <c r="AC8">
+        <v>61.3</v>
       </c>
       <c r="AD8">
         <v>10.1</v>
@@ -6287,8 +5894,8 @@
       <c r="AB9">
         <v>2957731</v>
       </c>
-      <c r="AC9" t="s">
-        <v>1533</v>
+      <c r="AC9">
+        <v>55.6</v>
       </c>
       <c r="AD9">
         <v>20.9</v>
@@ -6394,8 +6001,8 @@
       <c r="AB10">
         <v>25766605</v>
       </c>
-      <c r="AC10" t="s">
-        <v>1534</v>
+      <c r="AC10">
+        <v>65.5</v>
       </c>
       <c r="AD10">
         <v>23</v>
@@ -6501,8 +6108,8 @@
       <c r="AB11">
         <v>8877067</v>
       </c>
-      <c r="AC11" t="s">
-        <v>1535</v>
+      <c r="AC11">
+        <v>60.7</v>
       </c>
       <c r="AD11">
         <v>25.4</v>
@@ -6611,8 +6218,8 @@
       <c r="AB12">
         <v>10023318</v>
       </c>
-      <c r="AC12" t="s">
-        <v>1481</v>
+      <c r="AC12">
+        <v>66.5</v>
       </c>
       <c r="AD12">
         <v>13</v>
@@ -6718,8 +6325,8 @@
       <c r="AB13">
         <v>389482</v>
       </c>
-      <c r="AC13" t="s">
-        <v>1536</v>
+      <c r="AC13">
+        <v>74.59999999999999</v>
       </c>
       <c r="AD13">
         <v>14.8</v>
@@ -6825,8 +6432,8 @@
       <c r="AB14">
         <v>1501635</v>
       </c>
-      <c r="AC14" t="s">
-        <v>1537</v>
+      <c r="AC14">
+        <v>73.40000000000001</v>
       </c>
       <c r="AD14">
         <v>4.2</v>
@@ -6935,8 +6542,8 @@
       <c r="AB15">
         <v>167310838</v>
       </c>
-      <c r="AC15" t="s">
-        <v>1538</v>
+      <c r="AC15">
+        <v>59</v>
       </c>
       <c r="AD15">
         <v>8.800000000000001</v>
@@ -7045,8 +6652,8 @@
       <c r="AB16">
         <v>287025</v>
       </c>
-      <c r="AC16" t="s">
-        <v>1539</v>
+      <c r="AC16">
+        <v>65.2</v>
       </c>
       <c r="AD16">
         <v>27.5</v>
@@ -7152,8 +6759,8 @@
       <c r="AB17">
         <v>9466856</v>
       </c>
-      <c r="AC17" t="s">
-        <v>1540</v>
+      <c r="AC17">
+        <v>64.09999999999999</v>
       </c>
       <c r="AD17">
         <v>14.7</v>
@@ -7262,8 +6869,8 @@
       <c r="AB18">
         <v>11484055</v>
       </c>
-      <c r="AC18" t="s">
-        <v>1541</v>
+      <c r="AC18">
+        <v>53.6</v>
       </c>
       <c r="AD18">
         <v>24</v>
@@ -7372,8 +6979,8 @@
       <c r="AB19">
         <v>390353</v>
       </c>
-      <c r="AC19" t="s">
-        <v>1440</v>
+      <c r="AC19">
+        <v>65.09999999999999</v>
       </c>
       <c r="AD19">
         <v>26.3</v>
@@ -7482,8 +7089,8 @@
       <c r="AB20">
         <v>11801151</v>
       </c>
-      <c r="AC20" t="s">
-        <v>1542</v>
+      <c r="AC20">
+        <v>70.90000000000001</v>
       </c>
       <c r="AD20">
         <v>10.8</v>
@@ -7589,8 +7196,8 @@
       <c r="AB21">
         <v>727145</v>
       </c>
-      <c r="AC21" t="s">
-        <v>1543</v>
+      <c r="AC21">
+        <v>66.7</v>
       </c>
       <c r="AD21">
         <v>16</v>
@@ -7696,8 +7303,8 @@
       <c r="AB22">
         <v>11513100</v>
       </c>
-      <c r="AC22" t="s">
-        <v>1383</v>
+      <c r="AC22">
+        <v>71.8</v>
       </c>
       <c r="AD22">
         <v>17</v>
@@ -7803,8 +7410,8 @@
       <c r="AB23">
         <v>3301000</v>
       </c>
-      <c r="AC23" t="s">
-        <v>1544</v>
+      <c r="AC23">
+        <v>46.4</v>
       </c>
       <c r="AD23">
         <v>20.4</v>
@@ -7913,8 +7520,8 @@
       <c r="AB24">
         <v>2346179</v>
       </c>
-      <c r="AC24" t="s">
-        <v>1545</v>
+      <c r="AC24">
+        <v>70.8</v>
       </c>
       <c r="AD24">
         <v>19.5</v>
@@ -8023,8 +7630,8 @@
       <c r="AB25">
         <v>212559417</v>
       </c>
-      <c r="AC25" t="s">
-        <v>1546</v>
+      <c r="AC25">
+        <v>63.9</v>
       </c>
       <c r="AD25">
         <v>14.2</v>
@@ -8127,8 +7734,8 @@
       <c r="AB26">
         <v>433285</v>
       </c>
-      <c r="AC26" t="s">
-        <v>1547</v>
+      <c r="AC26">
+        <v>64.7</v>
       </c>
       <c r="AE26">
         <v>8</v>
@@ -8234,8 +7841,8 @@
       <c r="AB27">
         <v>6975761</v>
       </c>
-      <c r="AC27" t="s">
-        <v>1548</v>
+      <c r="AC27">
+        <v>55.4</v>
       </c>
       <c r="AD27">
         <v>20.2</v>
@@ -8344,8 +7951,8 @@
       <c r="AB28">
         <v>20321378</v>
       </c>
-      <c r="AC28" t="s">
-        <v>1549</v>
+      <c r="AC28">
+        <v>66.40000000000001</v>
       </c>
       <c r="AD28">
         <v>15</v>
@@ -8451,8 +8058,8 @@
       <c r="AB29">
         <v>11530580</v>
       </c>
-      <c r="AC29" t="s">
-        <v>1550</v>
+      <c r="AC29">
+        <v>79.2</v>
       </c>
       <c r="AD29">
         <v>13.6</v>
@@ -8561,8 +8168,8 @@
       <c r="AB30">
         <v>25716544</v>
       </c>
-      <c r="AC30" t="s">
-        <v>1432</v>
+      <c r="AC30">
+        <v>57</v>
       </c>
       <c r="AD30">
         <v>11.8</v>
@@ -8671,8 +8278,8 @@
       <c r="AB31">
         <v>483628</v>
       </c>
-      <c r="AC31" t="s">
-        <v>1551</v>
+      <c r="AC31">
+        <v>60.5</v>
       </c>
       <c r="AD31">
         <v>20.1</v>
@@ -8775,8 +8382,8 @@
       <c r="AB32">
         <v>16486542</v>
       </c>
-      <c r="AC32" t="s">
-        <v>1552</v>
+      <c r="AC32">
+        <v>82.3</v>
       </c>
       <c r="AD32">
         <v>17.1</v>
@@ -8885,8 +8492,8 @@
       <c r="AB33">
         <v>25876380</v>
       </c>
-      <c r="AC33" t="s">
-        <v>1553</v>
+      <c r="AC33">
+        <v>76.09999999999999</v>
       </c>
       <c r="AD33">
         <v>12.8</v>
@@ -8995,8 +8602,8 @@
       <c r="AB34">
         <v>36991981</v>
       </c>
-      <c r="AC34" t="s">
-        <v>1440</v>
+      <c r="AC34">
+        <v>65.09999999999999</v>
       </c>
       <c r="AD34">
         <v>12.8</v>
@@ -9102,8 +8709,8 @@
       <c r="AB35">
         <v>4745185</v>
       </c>
-      <c r="AC35" t="s">
-        <v>1420</v>
+      <c r="AC35">
+        <v>72</v>
       </c>
       <c r="AD35">
         <v>8.6</v>
@@ -9212,8 +8819,8 @@
       <c r="AB36">
         <v>15946876</v>
       </c>
-      <c r="AC36" t="s">
-        <v>1554</v>
+      <c r="AC36">
+        <v>70.7</v>
       </c>
       <c r="AE36">
         <v>63.5</v>
@@ -9319,8 +8926,8 @@
       <c r="AB37">
         <v>18952038</v>
       </c>
-      <c r="AC37" t="s">
-        <v>1555</v>
+      <c r="AC37">
+        <v>62.6</v>
       </c>
       <c r="AD37">
         <v>18.2</v>
@@ -9429,8 +9036,8 @@
       <c r="AB38">
         <v>1397715000</v>
       </c>
-      <c r="AC38" t="s">
-        <v>1556</v>
+      <c r="AC38">
+        <v>68</v>
       </c>
       <c r="AD38">
         <v>9.4</v>
@@ -9539,8 +9146,8 @@
       <c r="AB39">
         <v>50339443</v>
       </c>
-      <c r="AC39" t="s">
-        <v>1557</v>
+      <c r="AC39">
+        <v>68.8</v>
       </c>
       <c r="AD39">
         <v>14.4</v>
@@ -9643,8 +9250,8 @@
       <c r="AB40">
         <v>850886</v>
       </c>
-      <c r="AC40" t="s">
-        <v>1558</v>
+      <c r="AC40">
+        <v>43.3</v>
       </c>
       <c r="AE40">
         <v>219.6</v>
@@ -9747,8 +9354,8 @@
       <c r="AB41">
         <v>5380508</v>
       </c>
-      <c r="AC41" t="s">
-        <v>1559</v>
+      <c r="AC41">
+        <v>69.40000000000001</v>
       </c>
       <c r="AD41">
         <v>9</v>
@@ -9857,8 +9464,8 @@
       <c r="AB42">
         <v>5047561</v>
       </c>
-      <c r="AC42" t="s">
-        <v>1560</v>
+      <c r="AC42">
+        <v>62.1</v>
       </c>
       <c r="AD42">
         <v>13.6</v>
@@ -9967,8 +9574,8 @@
       <c r="AB43">
         <v>4067500</v>
       </c>
-      <c r="AC43" t="s">
-        <v>1561</v>
+      <c r="AC43">
+        <v>51.2</v>
       </c>
       <c r="AD43">
         <v>22</v>
@@ -10068,8 +9675,8 @@
       <c r="AB44">
         <v>11333483</v>
       </c>
-      <c r="AC44" t="s">
-        <v>1541</v>
+      <c r="AC44">
+        <v>53.6</v>
       </c>
       <c r="AF44">
         <v>1.64</v>
@@ -10169,8 +9776,8 @@
       <c r="AB45">
         <v>1198575</v>
       </c>
-      <c r="AC45" t="s">
-        <v>1509</v>
+      <c r="AC45">
+        <v>63.1</v>
       </c>
       <c r="AD45">
         <v>24.5</v>
@@ -10279,8 +9886,8 @@
       <c r="AB46">
         <v>10669709</v>
       </c>
-      <c r="AC46" t="s">
-        <v>1562</v>
+      <c r="AC46">
+        <v>60.6</v>
       </c>
       <c r="AD46">
         <v>14.9</v>
@@ -10389,8 +9996,8 @@
       <c r="AB47">
         <v>86790567</v>
       </c>
-      <c r="AC47" t="s">
-        <v>1563</v>
+      <c r="AC47">
+        <v>63.5</v>
       </c>
       <c r="AD47">
         <v>10.7</v>
@@ -10496,8 +10103,8 @@
       <c r="AB48">
         <v>5818553</v>
       </c>
-      <c r="AC48" t="s">
-        <v>1564</v>
+      <c r="AC48">
+        <v>62.2</v>
       </c>
       <c r="AD48">
         <v>32.4</v>
@@ -10603,8 +10210,8 @@
       <c r="AB49">
         <v>973560</v>
       </c>
-      <c r="AC49" t="s">
-        <v>1565</v>
+      <c r="AC49">
+        <v>60.2</v>
       </c>
       <c r="AE49">
         <v>37.9</v>
@@ -10805,8 +10412,8 @@
       <c r="AB51">
         <v>10738958</v>
       </c>
-      <c r="AC51" t="s">
-        <v>1566</v>
+      <c r="AC51">
+        <v>64.3</v>
       </c>
       <c r="AD51">
         <v>13</v>
@@ -10915,8 +10522,8 @@
       <c r="AB52">
         <v>17373662</v>
       </c>
-      <c r="AC52" t="s">
-        <v>1556</v>
+      <c r="AC52">
+        <v>68</v>
       </c>
       <c r="AE52">
         <v>34.4</v>
@@ -11019,8 +10626,8 @@
       <c r="AB53">
         <v>100388073</v>
       </c>
-      <c r="AC53" t="s">
-        <v>1544</v>
+      <c r="AC53">
+        <v>46.4</v>
       </c>
       <c r="AD53">
         <v>12.5</v>
@@ -11126,8 +10733,8 @@
       <c r="AB54">
         <v>6453553</v>
       </c>
-      <c r="AC54" t="s">
-        <v>1567</v>
+      <c r="AC54">
+        <v>59.1</v>
       </c>
       <c r="AD54">
         <v>18.1</v>
@@ -11233,8 +10840,8 @@
       <c r="AB55">
         <v>1355986</v>
       </c>
-      <c r="AC55" t="s">
-        <v>1418</v>
+      <c r="AC55">
+        <v>62</v>
       </c>
       <c r="AD55">
         <v>6.1</v>
@@ -11334,8 +10941,8 @@
       <c r="AB56">
         <v>6333135</v>
       </c>
-      <c r="AC56" t="s">
-        <v>1370</v>
+      <c r="AC56">
+        <v>78.40000000000001</v>
       </c>
       <c r="AE56">
         <v>83.7</v>
@@ -11441,8 +11048,8 @@
       <c r="AB57">
         <v>1331824</v>
       </c>
-      <c r="AC57" t="s">
-        <v>1568</v>
+      <c r="AC57">
+        <v>63.6</v>
       </c>
       <c r="AD57">
         <v>20.9</v>
@@ -11592,8 +11199,8 @@
       <c r="AB59">
         <v>112078730</v>
       </c>
-      <c r="AC59" t="s">
-        <v>1569</v>
+      <c r="AC59">
+        <v>79.59999999999999</v>
       </c>
       <c r="AD59">
         <v>7.5</v>
@@ -11702,8 +11309,8 @@
       <c r="AB60">
         <v>889953</v>
       </c>
-      <c r="AC60" t="s">
-        <v>1570</v>
+      <c r="AC60">
+        <v>57.6</v>
       </c>
       <c r="AD60">
         <v>24.2</v>
@@ -11809,8 +11416,8 @@
       <c r="AB61">
         <v>5520314</v>
       </c>
-      <c r="AC61" t="s">
-        <v>1567</v>
+      <c r="AC61">
+        <v>59.1</v>
       </c>
       <c r="AD61">
         <v>20.8</v>
@@ -11919,8 +11526,8 @@
       <c r="AB62">
         <v>67059887</v>
       </c>
-      <c r="AC62" t="s">
-        <v>1571</v>
+      <c r="AC62">
+        <v>55.1</v>
       </c>
       <c r="AD62">
         <v>24.2</v>
@@ -12029,8 +11636,8 @@
       <c r="AB63">
         <v>2172579</v>
       </c>
-      <c r="AC63" t="s">
-        <v>1572</v>
+      <c r="AC63">
+        <v>52.9</v>
       </c>
       <c r="AD63">
         <v>10.2</v>
@@ -12139,8 +11746,8 @@
       <c r="AB64">
         <v>2347706</v>
       </c>
-      <c r="AC64" t="s">
-        <v>1399</v>
+      <c r="AC64">
+        <v>59.4</v>
       </c>
       <c r="AD64">
         <v>9.4</v>
@@ -12249,8 +11856,8 @@
       <c r="AB65">
         <v>3720382</v>
       </c>
-      <c r="AC65" t="s">
-        <v>1573</v>
+      <c r="AC65">
+        <v>68.3</v>
       </c>
       <c r="AD65">
         <v>21.7</v>
@@ -12359,8 +11966,8 @@
       <c r="AB66">
         <v>83132799</v>
       </c>
-      <c r="AC66" t="s">
-        <v>1574</v>
+      <c r="AC66">
+        <v>60.8</v>
       </c>
       <c r="AD66">
         <v>11.5</v>
@@ -12469,8 +12076,8 @@
       <c r="AB67">
         <v>30792608</v>
       </c>
-      <c r="AC67" t="s">
-        <v>1575</v>
+      <c r="AC67">
+        <v>67.8</v>
       </c>
       <c r="AD67">
         <v>12.6</v>
@@ -12579,8 +12186,8 @@
       <c r="AB68">
         <v>10716322</v>
       </c>
-      <c r="AC68" t="s">
-        <v>1576</v>
+      <c r="AC68">
+        <v>51.8</v>
       </c>
       <c r="AD68">
         <v>26.2</v>
@@ -12787,8 +12394,8 @@
       <c r="AB70">
         <v>16604026</v>
       </c>
-      <c r="AC70" t="s">
-        <v>1577</v>
+      <c r="AC70">
+        <v>62.3</v>
       </c>
       <c r="AD70">
         <v>10.6</v>
@@ -12894,8 +12501,8 @@
       <c r="AB71">
         <v>12771246</v>
       </c>
-      <c r="AC71" t="s">
-        <v>1578</v>
+      <c r="AC71">
+        <v>61.5</v>
       </c>
       <c r="AD71">
         <v>10.8</v>
@@ -13001,8 +12608,8 @@
       <c r="AB72">
         <v>1920922</v>
       </c>
-      <c r="AC72" t="s">
-        <v>1420</v>
+      <c r="AC72">
+        <v>72</v>
       </c>
       <c r="AD72">
         <v>10.3</v>
@@ -13111,8 +12718,8 @@
       <c r="AB73">
         <v>782766</v>
       </c>
-      <c r="AC73" t="s">
-        <v>1579</v>
+      <c r="AC73">
+        <v>56.2</v>
       </c>
       <c r="AE73">
         <v>30.6</v>
@@ -13218,8 +12825,8 @@
       <c r="AB74">
         <v>11263077</v>
       </c>
-      <c r="AC74" t="s">
-        <v>1580</v>
+      <c r="AC74">
+        <v>67.2</v>
       </c>
       <c r="AE74">
         <v>42.7</v>
@@ -13360,8 +12967,8 @@
       <c r="AB76">
         <v>9746117</v>
       </c>
-      <c r="AC76" t="s">
-        <v>1557</v>
+      <c r="AC76">
+        <v>68.8</v>
       </c>
       <c r="AD76">
         <v>17.3</v>
@@ -13470,8 +13077,8 @@
       <c r="AB77">
         <v>9769949</v>
       </c>
-      <c r="AC77" t="s">
-        <v>1581</v>
+      <c r="AC77">
+        <v>56.5</v>
       </c>
       <c r="AD77">
         <v>23</v>
@@ -13577,8 +13184,8 @@
       <c r="AB78">
         <v>361313</v>
       </c>
-      <c r="AC78" t="s">
-        <v>1582</v>
+      <c r="AC78">
+        <v>75</v>
       </c>
       <c r="AD78">
         <v>23.3</v>
@@ -13687,8 +13294,8 @@
       <c r="AB79">
         <v>1366417754</v>
       </c>
-      <c r="AC79" t="s">
-        <v>1583</v>
+      <c r="AC79">
+        <v>49.3</v>
       </c>
       <c r="AD79">
         <v>11.2</v>
@@ -13797,8 +13404,8 @@
       <c r="AB80">
         <v>270203917</v>
       </c>
-      <c r="AC80" t="s">
-        <v>1584</v>
+      <c r="AC80">
+        <v>67.5</v>
       </c>
       <c r="AD80">
         <v>10.2</v>
@@ -13907,8 +13514,8 @@
       <c r="AB81">
         <v>82913906</v>
       </c>
-      <c r="AC81" t="s">
-        <v>1585</v>
+      <c r="AC81">
+        <v>44.7</v>
       </c>
       <c r="AD81">
         <v>7.4</v>
@@ -14017,8 +13624,8 @@
       <c r="AB82">
         <v>39309783</v>
       </c>
-      <c r="AC82" t="s">
-        <v>1586</v>
+      <c r="AC82">
+        <v>43</v>
       </c>
       <c r="AD82">
         <v>2</v>
@@ -14124,8 +13731,8 @@
       <c r="AB83">
         <v>5007069</v>
       </c>
-      <c r="AC83" t="s">
-        <v>1560</v>
+      <c r="AC83">
+        <v>62.1</v>
       </c>
       <c r="AD83">
         <v>18.3</v>
@@ -14234,8 +13841,8 @@
       <c r="AB84">
         <v>9053300</v>
       </c>
-      <c r="AC84" t="s">
-        <v>1587</v>
+      <c r="AC84">
+        <v>64</v>
       </c>
       <c r="AD84">
         <v>23.1</v>
@@ -14341,8 +13948,8 @@
       <c r="AB85">
         <v>60297396</v>
       </c>
-      <c r="AC85" t="s">
-        <v>1588</v>
+      <c r="AC85">
+        <v>49.6</v>
       </c>
       <c r="AD85">
         <v>24.3</v>
@@ -14451,8 +14058,8 @@
       <c r="AB86">
         <v>2948279</v>
       </c>
-      <c r="AC86" t="s">
-        <v>1589</v>
+      <c r="AC86">
+        <v>66</v>
       </c>
       <c r="AD86">
         <v>26.8</v>
@@ -14555,8 +14162,8 @@
       <c r="AB87">
         <v>126226568</v>
       </c>
-      <c r="AC87" t="s">
-        <v>1590</v>
+      <c r="AC87">
+        <v>61.7</v>
       </c>
       <c r="AD87">
         <v>11.9</v>
@@ -14665,8 +14272,8 @@
       <c r="AB88">
         <v>10101694</v>
       </c>
-      <c r="AC88" t="s">
-        <v>1468</v>
+      <c r="AC88">
+        <v>39.3</v>
       </c>
       <c r="AD88">
         <v>15.1</v>
@@ -14775,8 +14382,8 @@
       <c r="AB89">
         <v>18513930</v>
       </c>
-      <c r="AC89" t="s">
-        <v>1557</v>
+      <c r="AC89">
+        <v>68.8</v>
       </c>
       <c r="AD89">
         <v>11.7</v>
@@ -14885,8 +14492,8 @@
       <c r="AB90">
         <v>52573973</v>
       </c>
-      <c r="AC90" t="s">
-        <v>1591</v>
+      <c r="AC90">
+        <v>74.7</v>
       </c>
       <c r="AD90">
         <v>15.1</v>
@@ -15087,8 +14694,8 @@
       <c r="AB92">
         <v>4207083</v>
       </c>
-      <c r="AC92" t="s">
-        <v>1592</v>
+      <c r="AC92">
+        <v>73.5</v>
       </c>
       <c r="AD92">
         <v>1.4</v>
@@ -15197,8 +14804,8 @@
       <c r="AB93">
         <v>6456900</v>
       </c>
-      <c r="AC93" t="s">
-        <v>1593</v>
+      <c r="AC93">
+        <v>59.8</v>
       </c>
       <c r="AD93">
         <v>18</v>
@@ -15307,8 +14914,8 @@
       <c r="AB94">
         <v>7169455</v>
       </c>
-      <c r="AC94" t="s">
-        <v>1594</v>
+      <c r="AC94">
+        <v>78.5</v>
       </c>
       <c r="AD94">
         <v>12.9</v>
@@ -15417,8 +15024,8 @@
       <c r="AB95">
         <v>1912789</v>
       </c>
-      <c r="AC95" t="s">
-        <v>1595</v>
+      <c r="AC95">
+        <v>61.4</v>
       </c>
       <c r="AD95">
         <v>22.9</v>
@@ -15527,8 +15134,8 @@
       <c r="AB96">
         <v>6855713</v>
       </c>
-      <c r="AC96" t="s">
-        <v>1596</v>
+      <c r="AC96">
+        <v>47</v>
       </c>
       <c r="AD96">
         <v>15.3</v>
@@ -15634,8 +15241,8 @@
       <c r="AB97">
         <v>2125268</v>
       </c>
-      <c r="AC97" t="s">
-        <v>1597</v>
+      <c r="AC97">
+        <v>67.90000000000001</v>
       </c>
       <c r="AD97">
         <v>31.6</v>
@@ -15741,8 +15348,8 @@
       <c r="AB98">
         <v>4937374</v>
       </c>
-      <c r="AC98" t="s">
-        <v>1598</v>
+      <c r="AC98">
+        <v>76.3</v>
       </c>
       <c r="AD98">
         <v>12.9</v>
@@ -15845,8 +15452,8 @@
       <c r="AB99">
         <v>6777452</v>
       </c>
-      <c r="AC99" t="s">
-        <v>1599</v>
+      <c r="AC99">
+        <v>49.7</v>
       </c>
       <c r="AE99">
         <v>32.6</v>
@@ -16029,8 +15636,8 @@
       <c r="AB101">
         <v>2786844</v>
       </c>
-      <c r="AC101" t="s">
-        <v>1600</v>
+      <c r="AC101">
+        <v>61.6</v>
       </c>
       <c r="AD101">
         <v>16.9</v>
@@ -16139,8 +15746,8 @@
       <c r="AB102">
         <v>645397</v>
       </c>
-      <c r="AC102" t="s">
-        <v>1601</v>
+      <c r="AC102">
+        <v>59.3</v>
       </c>
       <c r="AD102">
         <v>26.5</v>
@@ -16249,8 +15856,8 @@
       <c r="AB103">
         <v>26969307</v>
       </c>
-      <c r="AC103" t="s">
-        <v>1602</v>
+      <c r="AC103">
+        <v>86.09999999999999</v>
       </c>
       <c r="AD103">
         <v>10.2</v>
@@ -16359,8 +15966,8 @@
       <c r="AB104">
         <v>18628747</v>
       </c>
-      <c r="AC104" t="s">
-        <v>1603</v>
+      <c r="AC104">
+        <v>76.7</v>
       </c>
       <c r="AD104">
         <v>17.3</v>
@@ -16469,8 +16076,8 @@
       <c r="AB105">
         <v>32447385</v>
       </c>
-      <c r="AC105" t="s">
-        <v>1566</v>
+      <c r="AC105">
+        <v>64.3</v>
       </c>
       <c r="AD105">
         <v>12</v>
@@ -16573,8 +16180,8 @@
       <c r="AB106">
         <v>530953</v>
       </c>
-      <c r="AC106" t="s">
-        <v>1604</v>
+      <c r="AC106">
+        <v>69.8</v>
       </c>
       <c r="AD106">
         <v>19.5</v>
@@ -16683,8 +16290,8 @@
       <c r="AB107">
         <v>19658031</v>
       </c>
-      <c r="AC107" t="s">
-        <v>1545</v>
+      <c r="AC107">
+        <v>70.8</v>
       </c>
       <c r="AD107">
         <v>11.6</v>
@@ -16793,8 +16400,8 @@
       <c r="AB108">
         <v>502653</v>
       </c>
-      <c r="AC108" t="s">
-        <v>1581</v>
+      <c r="AC108">
+        <v>56.5</v>
       </c>
       <c r="AD108">
         <v>26.2</v>
@@ -16995,8 +16602,8 @@
       <c r="AB110">
         <v>4525696</v>
       </c>
-      <c r="AC110" t="s">
-        <v>1605</v>
+      <c r="AC110">
+        <v>45.9</v>
       </c>
       <c r="AE110">
         <v>67</v>
@@ -17102,8 +16709,8 @@
       <c r="AB111">
         <v>1265711</v>
       </c>
-      <c r="AC111" t="s">
-        <v>1606</v>
+      <c r="AC111">
+        <v>58.3</v>
       </c>
       <c r="AD111">
         <v>19.1</v>
@@ -17209,8 +16816,8 @@
       <c r="AB112">
         <v>126014024</v>
       </c>
-      <c r="AC112" t="s">
-        <v>1535</v>
+      <c r="AC112">
+        <v>60.7</v>
       </c>
       <c r="AD112">
         <v>13.1</v>
@@ -17414,8 +17021,8 @@
       <c r="AB114">
         <v>2657637</v>
       </c>
-      <c r="AC114" t="s">
-        <v>1607</v>
+      <c r="AC114">
+        <v>43.1</v>
       </c>
       <c r="AD114">
         <v>17.7</v>
@@ -17589,8 +17196,8 @@
       <c r="AB116">
         <v>3225167</v>
       </c>
-      <c r="AC116" t="s">
-        <v>1608</v>
+      <c r="AC116">
+        <v>59.7</v>
       </c>
       <c r="AD116">
         <v>16.8</v>
@@ -17699,8 +17306,8 @@
       <c r="AB117">
         <v>622137</v>
       </c>
-      <c r="AC117" t="s">
-        <v>1609</v>
+      <c r="AC117">
+        <v>54.4</v>
       </c>
       <c r="AE117">
         <v>22.2</v>
@@ -17806,8 +17413,8 @@
       <c r="AB118">
         <v>36910560</v>
       </c>
-      <c r="AC118" t="s">
-        <v>1610</v>
+      <c r="AC118">
+        <v>45.3</v>
       </c>
       <c r="AD118">
         <v>21.9</v>
@@ -17916,8 +17523,8 @@
       <c r="AB119">
         <v>30366036</v>
       </c>
-      <c r="AC119" t="s">
-        <v>1611</v>
+      <c r="AC119">
+        <v>78.09999999999999</v>
       </c>
       <c r="AD119">
         <v>0</v>
@@ -18026,8 +17633,8 @@
       <c r="AB120">
         <v>54045420</v>
       </c>
-      <c r="AC120" t="s">
-        <v>1590</v>
+      <c r="AC120">
+        <v>61.7</v>
       </c>
       <c r="AD120">
         <v>5.4</v>
@@ -18127,8 +17734,8 @@
       <c r="AB121">
         <v>2494530</v>
       </c>
-      <c r="AC121" t="s">
-        <v>1612</v>
+      <c r="AC121">
+        <v>59.5</v>
       </c>
       <c r="AD121">
         <v>27.1</v>
@@ -18278,8 +17885,8 @@
       <c r="AB123">
         <v>28608710</v>
       </c>
-      <c r="AC123" t="s">
-        <v>1613</v>
+      <c r="AC123">
+        <v>83.8</v>
       </c>
       <c r="AD123">
         <v>20.7</v>
@@ -18385,8 +17992,8 @@
       <c r="AB124">
         <v>17332850</v>
       </c>
-      <c r="AC124" t="s">
-        <v>1568</v>
+      <c r="AC124">
+        <v>63.6</v>
       </c>
       <c r="AD124">
         <v>23</v>
@@ -18495,8 +18102,8 @@
       <c r="AB125">
         <v>4841000</v>
       </c>
-      <c r="AC125" t="s">
-        <v>1614</v>
+      <c r="AC125">
+        <v>69.90000000000001</v>
       </c>
       <c r="AD125">
         <v>29</v>
@@ -18605,8 +18212,8 @@
       <c r="AB126">
         <v>6545502</v>
       </c>
-      <c r="AC126" t="s">
-        <v>1549</v>
+      <c r="AC126">
+        <v>66.40000000000001</v>
       </c>
       <c r="AD126">
         <v>15.6</v>
@@ -18715,8 +18322,8 @@
       <c r="AB127">
         <v>23310715</v>
       </c>
-      <c r="AC127" t="s">
-        <v>1420</v>
+      <c r="AC127">
+        <v>72</v>
       </c>
       <c r="AD127">
         <v>11.8</v>
@@ -18825,8 +18432,8 @@
       <c r="AB128">
         <v>200963599</v>
       </c>
-      <c r="AC128" t="s">
-        <v>1572</v>
+      <c r="AC128">
+        <v>52.9</v>
       </c>
       <c r="AD128">
         <v>1.5</v>
@@ -18923,8 +18530,8 @@
       <c r="AB129">
         <v>25666161</v>
       </c>
-      <c r="AC129" t="s">
-        <v>1615</v>
+      <c r="AC129">
+        <v>80.40000000000001</v>
       </c>
       <c r="AF129">
         <v>2.74</v>
@@ -19068,8 +18675,8 @@
       <c r="AB131">
         <v>5347896</v>
       </c>
-      <c r="AC131" t="s">
-        <v>1616</v>
+      <c r="AC131">
+        <v>63.8</v>
       </c>
       <c r="AD131">
         <v>23.9</v>
@@ -19178,8 +18785,8 @@
       <c r="AB132">
         <v>5266535</v>
       </c>
-      <c r="AC132" t="s">
-        <v>1617</v>
+      <c r="AC132">
+        <v>72.40000000000001</v>
       </c>
       <c r="AD132">
         <v>2.5</v>
@@ -19288,8 +18895,8 @@
       <c r="AB133">
         <v>216565318</v>
       </c>
-      <c r="AC133" t="s">
-        <v>1618</v>
+      <c r="AC133">
+        <v>52.6</v>
       </c>
       <c r="AD133">
         <v>9.199999999999999</v>
@@ -19510,8 +19117,8 @@
       <c r="AB136">
         <v>4246439</v>
       </c>
-      <c r="AC136" t="s">
-        <v>1619</v>
+      <c r="AC136">
+        <v>66.59999999999999</v>
       </c>
       <c r="AE136">
         <v>37.2</v>
@@ -19617,8 +19224,8 @@
       <c r="AB137">
         <v>8776109</v>
       </c>
-      <c r="AC137" t="s">
-        <v>1620</v>
+      <c r="AC137">
+        <v>47.2</v>
       </c>
       <c r="AD137">
         <v>13.6</v>
@@ -19727,8 +19334,8 @@
       <c r="AB138">
         <v>7044636</v>
       </c>
-      <c r="AC138" t="s">
-        <v>1621</v>
+      <c r="AC138">
+        <v>72.09999999999999</v>
       </c>
       <c r="AD138">
         <v>10</v>
@@ -19837,8 +19444,8 @@
       <c r="AB139">
         <v>32510453</v>
       </c>
-      <c r="AC139" t="s">
-        <v>1622</v>
+      <c r="AC139">
+        <v>77.59999999999999</v>
       </c>
       <c r="AD139">
         <v>14.3</v>
@@ -19947,8 +19554,8 @@
       <c r="AB140">
         <v>108116615</v>
       </c>
-      <c r="AC140" t="s">
-        <v>1623</v>
+      <c r="AC140">
+        <v>59.6</v>
       </c>
       <c r="AD140">
         <v>14</v>
@@ -20057,8 +19664,8 @@
       <c r="AB141">
         <v>37970874</v>
       </c>
-      <c r="AC141" t="s">
-        <v>1624</v>
+      <c r="AC141">
+        <v>56.7</v>
       </c>
       <c r="AD141">
         <v>17.4</v>
@@ -20167,8 +19774,8 @@
       <c r="AB142">
         <v>10269417</v>
       </c>
-      <c r="AC142" t="s">
-        <v>1625</v>
+      <c r="AC142">
+        <v>58.8</v>
       </c>
       <c r="AD142">
         <v>22.8</v>
@@ -20274,8 +19881,8 @@
       <c r="AB143">
         <v>2832067</v>
       </c>
-      <c r="AC143" t="s">
-        <v>1626</v>
+      <c r="AC143">
+        <v>86.8</v>
       </c>
       <c r="AD143">
         <v>14.7</v>
@@ -20384,8 +19991,8 @@
       <c r="AB144">
         <v>19356544</v>
       </c>
-      <c r="AC144" t="s">
-        <v>1627</v>
+      <c r="AC144">
+        <v>54.7</v>
       </c>
       <c r="AD144">
         <v>14.6</v>
@@ -20494,8 +20101,8 @@
       <c r="AB145">
         <v>144373535</v>
       </c>
-      <c r="AC145" t="s">
-        <v>1628</v>
+      <c r="AC145">
+        <v>61.8</v>
       </c>
       <c r="AD145">
         <v>11.4</v>
@@ -20601,8 +20208,8 @@
       <c r="AB146">
         <v>12626950</v>
       </c>
-      <c r="AC146" t="s">
-        <v>1629</v>
+      <c r="AC146">
+        <v>83.7</v>
       </c>
       <c r="AD146">
         <v>14.3</v>
@@ -20800,8 +20407,8 @@
       <c r="AB148">
         <v>182790</v>
       </c>
-      <c r="AC148" t="s">
-        <v>1630</v>
+      <c r="AC148">
+        <v>67.09999999999999</v>
       </c>
       <c r="AD148">
         <v>18.2</v>
@@ -20904,8 +20511,8 @@
       <c r="AB149">
         <v>100455</v>
       </c>
-      <c r="AC149" t="s">
-        <v>1631</v>
+      <c r="AC149">
+        <v>65.90000000000001</v>
       </c>
       <c r="AD149">
         <v>25.4</v>
@@ -21011,8 +20618,8 @@
       <c r="AB150">
         <v>202506</v>
       </c>
-      <c r="AC150" t="s">
-        <v>1417</v>
+      <c r="AC150">
+        <v>43.7</v>
       </c>
       <c r="AD150">
         <v>25.5</v>
@@ -21210,8 +20817,8 @@
       <c r="AB153">
         <v>34268528</v>
       </c>
-      <c r="AC153" t="s">
-        <v>1632</v>
+      <c r="AC153">
+        <v>55.9</v>
       </c>
       <c r="AD153">
         <v>8.9</v>
@@ -21320,8 +20927,8 @@
       <c r="AB154">
         <v>16296364</v>
       </c>
-      <c r="AC154" t="s">
-        <v>1633</v>
+      <c r="AC154">
+        <v>45.7</v>
       </c>
       <c r="AD154">
         <v>16.3</v>
@@ -21430,8 +21037,8 @@
       <c r="AB155">
         <v>6944975</v>
       </c>
-      <c r="AC155" t="s">
-        <v>1634</v>
+      <c r="AC155">
+        <v>54.9</v>
       </c>
       <c r="AD155">
         <v>18.6</v>
@@ -21641,8 +21248,8 @@
       <c r="AB157">
         <v>7813215</v>
       </c>
-      <c r="AC157" t="s">
-        <v>1635</v>
+      <c r="AC157">
+        <v>57.9</v>
       </c>
       <c r="AD157">
         <v>8.6</v>
@@ -21742,8 +21349,8 @@
       <c r="AB158">
         <v>5703569</v>
       </c>
-      <c r="AC158" t="s">
-        <v>1636</v>
+      <c r="AC158">
+        <v>70.5</v>
       </c>
       <c r="AD158">
         <v>13.1</v>
@@ -21852,8 +21459,8 @@
       <c r="AB159">
         <v>5454073</v>
       </c>
-      <c r="AC159" t="s">
-        <v>1612</v>
+      <c r="AC159">
+        <v>59.5</v>
       </c>
       <c r="AD159">
         <v>18.7</v>
@@ -21962,8 +21569,8 @@
       <c r="AB160">
         <v>2087946</v>
       </c>
-      <c r="AC160" t="s">
-        <v>1637</v>
+      <c r="AC160">
+        <v>58.4</v>
       </c>
       <c r="AD160">
         <v>18.6</v>
@@ -22063,8 +21670,8 @@
       <c r="AB161">
         <v>669823</v>
       </c>
-      <c r="AC161" t="s">
-        <v>1613</v>
+      <c r="AC161">
+        <v>83.8</v>
       </c>
       <c r="AD161">
         <v>29.5</v>
@@ -22161,8 +21768,8 @@
       <c r="AB162">
         <v>15442905</v>
       </c>
-      <c r="AC162" t="s">
-        <v>1638</v>
+      <c r="AC162">
+        <v>47.4</v>
       </c>
       <c r="AD162">
         <v>0</v>
@@ -22265,8 +21872,8 @@
       <c r="AB163">
         <v>58558270</v>
       </c>
-      <c r="AC163" t="s">
-        <v>1639</v>
+      <c r="AC163">
+        <v>56</v>
       </c>
       <c r="AD163">
         <v>27.5</v>
@@ -22375,8 +21982,8 @@
       <c r="AB164">
         <v>51709098</v>
       </c>
-      <c r="AC164" t="s">
-        <v>1640</v>
+      <c r="AC164">
+        <v>63</v>
       </c>
       <c r="AD164">
         <v>15.6</v>
@@ -22470,8 +22077,8 @@
       <c r="AB165">
         <v>11062113</v>
       </c>
-      <c r="AC165" t="s">
-        <v>1617</v>
+      <c r="AC165">
+        <v>72.40000000000001</v>
       </c>
       <c r="AE165">
         <v>31.4</v>
@@ -22577,8 +22184,8 @@
       <c r="AB166">
         <v>47076781</v>
       </c>
-      <c r="AC166" t="s">
-        <v>1641</v>
+      <c r="AC166">
+        <v>57.5</v>
       </c>
       <c r="AD166">
         <v>14.2</v>
@@ -22687,8 +22294,8 @@
       <c r="AB167">
         <v>21803000</v>
       </c>
-      <c r="AC167" t="s">
-        <v>1642</v>
+      <c r="AC167">
+        <v>53.9</v>
       </c>
       <c r="AD167">
         <v>11.9</v>
@@ -22797,8 +22404,8 @@
       <c r="AB168">
         <v>42813238</v>
       </c>
-      <c r="AC168" t="s">
-        <v>1493</v>
+      <c r="AC168">
+        <v>48.4</v>
       </c>
       <c r="AD168">
         <v>8</v>
@@ -22904,8 +22511,8 @@
       <c r="AB169">
         <v>581372</v>
       </c>
-      <c r="AC169" t="s">
-        <v>1643</v>
+      <c r="AC169">
+        <v>51.1</v>
       </c>
       <c r="AD169">
         <v>19.5</v>
@@ -23011,8 +22618,8 @@
       <c r="AB170">
         <v>10285453</v>
       </c>
-      <c r="AC170" t="s">
-        <v>1644</v>
+      <c r="AC170">
+        <v>64.59999999999999</v>
       </c>
       <c r="AD170">
         <v>27.9</v>
@@ -23118,8 +22725,8 @@
       <c r="AB171">
         <v>8574832</v>
       </c>
-      <c r="AC171" t="s">
-        <v>1573</v>
+      <c r="AC171">
+        <v>68.3</v>
       </c>
       <c r="AD171">
         <v>10.1</v>
@@ -23228,8 +22835,8 @@
       <c r="AB172">
         <v>17070135</v>
       </c>
-      <c r="AC172" t="s">
-        <v>1645</v>
+      <c r="AC172">
+        <v>44.1</v>
       </c>
       <c r="AD172">
         <v>14.2</v>
@@ -23338,8 +22945,8 @@
       <c r="AB173">
         <v>9321018</v>
       </c>
-      <c r="AC173" t="s">
-        <v>1646</v>
+      <c r="AC173">
+        <v>42</v>
       </c>
       <c r="AD173">
         <v>9.800000000000001</v>
@@ -23448,8 +23055,8 @@
       <c r="AB174">
         <v>58005463</v>
       </c>
-      <c r="AC174" t="s">
-        <v>1647</v>
+      <c r="AC174">
+        <v>83.40000000000001</v>
       </c>
       <c r="AD174">
         <v>11.5</v>
@@ -23558,8 +23165,8 @@
       <c r="AB175">
         <v>69625582</v>
       </c>
-      <c r="AC175" t="s">
-        <v>1648</v>
+      <c r="AC175">
+        <v>67.3</v>
       </c>
       <c r="AD175">
         <v>14.9</v>
@@ -23668,8 +23275,8 @@
       <c r="AB176">
         <v>3500000</v>
       </c>
-      <c r="AC176" t="s">
-        <v>1648</v>
+      <c r="AC176">
+        <v>67.3</v>
       </c>
       <c r="AD176">
         <v>25</v>
@@ -23778,8 +23385,8 @@
       <c r="AB177">
         <v>8082366</v>
       </c>
-      <c r="AC177" t="s">
-        <v>1622</v>
+      <c r="AC177">
+        <v>77.59999999999999</v>
       </c>
       <c r="AD177">
         <v>16.9</v>
@@ -23879,8 +23486,8 @@
       <c r="AB178">
         <v>100209</v>
       </c>
-      <c r="AC178" t="s">
-        <v>1593</v>
+      <c r="AC178">
+        <v>59.8</v>
       </c>
       <c r="AD178">
         <v>22.3</v>
@@ -23989,8 +23596,8 @@
       <c r="AB179">
         <v>1394973</v>
       </c>
-      <c r="AC179" t="s">
-        <v>1649</v>
+      <c r="AC179">
+        <v>60</v>
       </c>
       <c r="AD179">
         <v>19.5</v>
@@ -24099,8 +23706,8 @@
       <c r="AB180">
         <v>11694719</v>
       </c>
-      <c r="AC180" t="s">
-        <v>1650</v>
+      <c r="AC180">
+        <v>46.1</v>
       </c>
       <c r="AD180">
         <v>21.1</v>
@@ -24209,8 +23816,8 @@
       <c r="AB181">
         <v>83429615</v>
       </c>
-      <c r="AC181" t="s">
-        <v>1651</v>
+      <c r="AC181">
+        <v>52.8</v>
       </c>
       <c r="AD181">
         <v>17.9</v>
@@ -24313,8 +23920,8 @@
       <c r="AB182">
         <v>5942089</v>
       </c>
-      <c r="AC182" t="s">
-        <v>1652</v>
+      <c r="AC182">
+        <v>64.5</v>
       </c>
       <c r="AF182">
         <v>3.91</v>
@@ -24485,8 +24092,8 @@
       <c r="AB184">
         <v>44269594</v>
       </c>
-      <c r="AC184" t="s">
-        <v>1653</v>
+      <c r="AC184">
+        <v>70.3</v>
       </c>
       <c r="AD184">
         <v>11.7</v>
@@ -24595,8 +24202,8 @@
       <c r="AB185">
         <v>44385155</v>
       </c>
-      <c r="AC185" t="s">
-        <v>1654</v>
+      <c r="AC185">
+        <v>54.2</v>
       </c>
       <c r="AD185">
         <v>20.1</v>
@@ -24702,8 +24309,8 @@
       <c r="AB186">
         <v>9770529</v>
       </c>
-      <c r="AC186" t="s">
-        <v>1655</v>
+      <c r="AC186">
+        <v>82.09999999999999</v>
       </c>
       <c r="AD186">
         <v>0.1</v>
@@ -24812,8 +24419,8 @@
       <c r="AB187">
         <v>66834405</v>
       </c>
-      <c r="AC187" t="s">
-        <v>1656</v>
+      <c r="AC187">
+        <v>62.8</v>
       </c>
       <c r="AD187">
         <v>25.5</v>
@@ -24919,8 +24526,8 @@
       <c r="AB188">
         <v>328239523</v>
       </c>
-      <c r="AC188" t="s">
-        <v>1418</v>
+      <c r="AC188">
+        <v>62</v>
       </c>
       <c r="AD188">
         <v>9.6</v>
@@ -25029,8 +24636,8 @@
       <c r="AB189">
         <v>3461734</v>
       </c>
-      <c r="AC189" t="s">
-        <v>1587</v>
+      <c r="AC189">
+        <v>64</v>
       </c>
       <c r="AD189">
         <v>20.1</v>
@@ -25133,8 +24740,8 @@
       <c r="AB190">
         <v>33580650</v>
       </c>
-      <c r="AC190" t="s">
-        <v>1440</v>
+      <c r="AC190">
+        <v>65.09999999999999</v>
       </c>
       <c r="AD190">
         <v>14.8</v>
@@ -25240,8 +24847,8 @@
       <c r="AB191">
         <v>299882</v>
       </c>
-      <c r="AC191" t="s">
-        <v>1614</v>
+      <c r="AC191">
+        <v>69.90000000000001</v>
       </c>
       <c r="AD191">
         <v>17.8</v>
@@ -25350,8 +24957,8 @@
       <c r="AB192">
         <v>28515829</v>
       </c>
-      <c r="AC192" t="s">
-        <v>1608</v>
+      <c r="AC192">
+        <v>59.7</v>
       </c>
       <c r="AE192">
         <v>73.3</v>
@@ -25457,8 +25064,8 @@
       <c r="AB193">
         <v>96462106</v>
       </c>
-      <c r="AC193" t="s">
-        <v>1657</v>
+      <c r="AC193">
+        <v>77.40000000000001</v>
       </c>
       <c r="AD193">
         <v>19.1</v>
@@ -25564,8 +25171,8 @@
       <c r="AB194">
         <v>29161922</v>
       </c>
-      <c r="AC194" t="s">
-        <v>1658</v>
+      <c r="AC194">
+        <v>38</v>
       </c>
       <c r="AE194">
         <v>26.6</v>
@@ -25671,8 +25278,8 @@
       <c r="AB195">
         <v>17861030</v>
       </c>
-      <c r="AC195" t="s">
-        <v>1536</v>
+      <c r="AC195">
+        <v>74.59999999999999</v>
       </c>
       <c r="AD195">
         <v>16.2</v>
@@ -25775,8 +25382,8 @@
       <c r="AB196">
         <v>14645468</v>
       </c>
-      <c r="AC196" t="s">
-        <v>1659</v>
+      <c r="AC196">
+        <v>83.09999999999999</v>
       </c>
       <c r="AD196">
         <v>20.7</v>

</xml_diff>